<commit_message>
made exploratory figures & updates models
</commit_message>
<xml_diff>
--- a/data/raw_lab_analyses/ELA_AMBIENT_FISH-EXCRETION-DOC_2022/ELA_AMBIENT_FISHreruns_DOC.xlsx
+++ b/data/raw_lab_analyses/ELA_AMBIENT_FISH-EXCRETION-DOC_2022/ELA_AMBIENT_FISHreruns_DOC.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trentu-my.sharepoint.com/personal/sandraklemet_trentu_ca/Documents/Documents/Etudes/Trent/Xenopoulos lab/Projects/11-DOC-ELA_animal-excretion/data/raw_lab_analyses/ELA_AMBIENT_FISH-EXCRETION-DOC_2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38D7C0C2-6BB6-414B-8389-79EC9351515E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{38D7C0C2-6BB6-414B-8389-79EC9351515E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D22AA68-C061-4CEE-8A6E-592F28F35A7B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELA_AMBIENT_DOC_2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="66">
   <si>
     <t>[Header]</t>
   </si>
@@ -215,12 +228,15 @@
   </si>
   <si>
     <t>14/04/2023 15:33:23</t>
+  </si>
+  <si>
+    <t>Detection limit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -759,9 +775,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -799,7 +815,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -905,7 +921,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1047,17 +1063,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1065,6 +1083,13 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1">
+        <f>AVERAGE(I15,I17,I36)</f>
+        <v>0.10049666666666668</v>
+      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">

</xml_diff>